<commit_message>
Added chat categories for fizzeled spells, spells that are on cooldown, and when the cooldownlist is full
FILES MODIFIED

BattleManager.cs

NOTES

So I've been having this problem where sometimes when unity wont see any data from a text asset. this usually happens after re-exporting an excel sheet, but sometimes isn't even fixed by creating a new excel, or even a new text file with all the text. Hit me up if anyone knows anything!
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/chatDatabase.xlsx
+++ b/Typocrypha/Assets/excel/chatDatabase.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>NEW_CATEGORY</t>
   </si>
@@ -39,12 +39,6 @@
     <t>Exodia, Obliterate!</t>
   </si>
   <si>
-    <t>I have the power of God AND anime on my side!</t>
-  </si>
-  <si>
-    <t>WHAT AM I FIGHTING FOR!?!?!?</t>
-  </si>
-  <si>
     <t>botch</t>
   </si>
   <si>
@@ -88,6 +82,30 @@
   </si>
   <si>
     <t>It'sa me, tanooki!</t>
+  </si>
+  <si>
+    <t>I can be your angle…. or yuor devil</t>
+  </si>
+  <si>
+    <t>All your base are belong to us!</t>
+  </si>
+  <si>
+    <t>fizzle</t>
+  </si>
+  <si>
+    <t>oncooldown</t>
+  </si>
+  <si>
+    <t>cooldownlistfull</t>
+  </si>
+  <si>
+    <t>Wow, I was WAY off…</t>
+  </si>
+  <si>
+    <t>Oh no, it's on cooldown!</t>
+  </si>
+  <si>
+    <t>My cooldown list is full!</t>
   </si>
 </sst>
 </file>
@@ -405,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,7 +472,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -462,7 +480,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -470,7 +488,7 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -478,7 +496,7 @@
         <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -486,47 +504,47 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>100</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
         <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -534,52 +552,100 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>10</v>
       </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>0</v>
-      </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
         <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>100</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed Spell Dictionary, Fixed Keys, Added Spell Diagram, etc.
- Changed spell dictionary words
- Fixed key button positions/text
- Added spell cast diagram
- Added enemy lines
- Changed dialogue for playtest
- Changed Spellbook button graphics
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/chatDatabase.xlsx
+++ b/Typocrypha/Assets/excel/chatDatabase.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>NEW_CATEGORY</t>
   </si>
@@ -106,12 +106,30 @@
   </si>
   <si>
     <t>My cooldown list is full!</t>
+  </si>
+  <si>
+    <t>ijiraq_1</t>
+  </si>
+  <si>
+    <t>changeling_1</t>
+  </si>
+  <si>
+    <t>doppelganger_1</t>
+  </si>
+  <si>
+    <t>THE ARCTIC WINDS ARE HOWLING . . .</t>
+  </si>
+  <si>
+    <t>NananaNaNAH! Tag, you're it!</t>
+  </si>
+  <si>
+    <t>I AM SASUN, GOD OF DESTRUCTION.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -422,20 +440,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="71.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="71.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,7 +461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -451,7 +469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -459,7 +477,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -467,7 +485,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>15</v>
       </c>
@@ -475,7 +493,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
@@ -483,7 +501,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -491,7 +509,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>100</v>
       </c>
@@ -499,7 +517,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -507,7 +525,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>100</v>
       </c>
@@ -515,7 +533,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -523,7 +541,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>100</v>
       </c>
@@ -531,7 +549,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -539,7 +557,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>100</v>
       </c>
@@ -547,7 +565,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -555,7 +573,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>50</v>
       </c>
@@ -563,7 +581,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>25</v>
       </c>
@@ -571,7 +589,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -579,7 +597,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10</v>
       </c>
@@ -587,7 +605,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>15</v>
       </c>
@@ -595,7 +613,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -603,7 +621,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10</v>
       </c>
@@ -611,7 +629,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
@@ -619,7 +637,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>10</v>
       </c>
@@ -627,7 +645,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -635,7 +653,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>100</v>
       </c>
@@ -643,8 +661,56 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>100</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>100</v>
+      </c>
+      <c r="B30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>100</v>
+      </c>
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor Stat Tweaks + Clarke's in
one scene wonder clarke in the doppelganger fight
</commit_message>
<xml_diff>
--- a/Typocrypha/Assets/excel/chatDatabase.xlsx
+++ b/Typocrypha/Assets/excel/chatDatabase.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117FA4FB-24BA-40F4-8146-4FFF013A3651}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>NEW_CATEGORY</t>
   </si>
@@ -123,13 +124,25 @@
     <t>NananaNaNAH! Tag, you're it!</t>
   </si>
   <si>
-    <t>I AM SASUN, GOD OF DESTRUCTION.</t>
+    <t>Bear witness to my power!</t>
+  </si>
+  <si>
+    <t>bunbuku_1</t>
+  </si>
+  <si>
+    <t>I'm on fire, baby!</t>
+  </si>
+  <si>
+    <t>wech_1</t>
+  </si>
+  <si>
+    <t>Please go away . . .</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -440,11 +453,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,7 +711,7 @@
         <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -706,11 +719,43 @@
         <v>100</v>
       </c>
       <c r="B32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>100</v>
+      </c>
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>100</v>
+      </c>
+      <c r="B36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>